<commit_message>
update optimisation data for fasttree
</commit_message>
<xml_diff>
--- a/ft_models.xlsx
+++ b/ft_models.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roblanfear/Documents/github/sarscov2phylo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3C4D4529-4E6B-A248-9265-1B8D1239135D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93324425-F0CA-AD45-AE42-B033ECDA46D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="7680" windowWidth="21160" windowHeight="16480"/>
+    <workbookView xWindow="5720" yWindow="460" windowWidth="21160" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ft_models" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="103">
   <si>
     <t>Iteration</t>
   </si>
@@ -299,12 +300,42 @@
   </si>
   <si>
     <t>/usr/bin/time -o 6.18.mem.txt -v fasttree -sprlength 20 -refresh 0.999 -topm 1.5 -close 0.5 -nosupport -nt -gamma -log 6.18.txt global.fa &gt; 6.18.tree</t>
+  </si>
+  <si>
+    <t>/usr/bin/time -o 7.1.mem.txt -v fasttree -sprlength 20 -refresh 0.8 -topm 1.6 -close 0.75 -nosupport -nt -gamma global.fa &gt; 7.1.tree</t>
+  </si>
+  <si>
+    <t>/usr/bin/time -o 7.2.mem.txt -v fasttree -sprlength 20 -refresh 0.8 -topm 1.8 -close 0.75 -nosupport -nt -gamma global.fa &gt; 7.2.tree</t>
+  </si>
+  <si>
+    <t>/usr/bin/time -o 7.3.mem.txt -v fasttree -sprlength 20 -refresh 0.8 -topm 2.0 -close 0.75 -nosupport -nt -gamma global.fa &gt; 7.3.tree</t>
+  </si>
+  <si>
+    <t>/usr/bin/time -o 7.4.mem.txt -v fasttree -sprlength 20 -refresh 0.8 -topm 2.25 -close 0.75 -nosupport -nt -gamma global.fa &gt; 7.4.tree</t>
+  </si>
+  <si>
+    <t>/usr/bin/time -o 7.5.mem.txt -v fasttree -sprlength 20 -refresh 0.8 -topm 2.5 -close 0.75 -nosupport -nt -gamma global.fa &gt; 7.5.tree</t>
+  </si>
+  <si>
+    <t>/usr/bin/time -o 8.3.mem.txt -v fasttree -sprlength 20 -refresh 0.8 -topm 2.25 -close 0.75 -2nd -nosupport -nt -gamma global.fa &gt; 8.3.tree</t>
+  </si>
+  <si>
+    <t>/usr/bin/time -o 8.1.mem.txt -v fasttree -sprlength 20 -refresh 0.8 -topm 2.25 -close 0.75 -nt -gamma global.fa &gt; 8.1.tree</t>
+  </si>
+  <si>
+    <t>/usr/bin/time -o 8.2.mem.txt -v fasttree -sprlength 20 -refresh 0.8 -topm 2.25 -close 0.75 -bionj -nosupport -nt -gamma global.fa &gt; 8.2.tree</t>
+  </si>
+  <si>
+    <t>/usr/bin/time -o 8.4.mem.txt -v fasttree -sprlength 20 -refresh 0.8 -topm 2.25 -close 0.75 -bionj -2nd -nosupport -nt -gamma global.fa &gt; 8.4.tree</t>
+  </si>
+  <si>
+    <t>/usr/bin/time -o 8.5.mem.txt -v fasttree -sprlength 20 -refresh 0.8 -topm 2.25 -close 0.75 -fastest -bionj -nosupport -nt -gamma global.fa &gt; 8.5.tree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1146,11 +1177,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J60"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1237,7 +1268,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F50" si="0">C3-$C$2</f>
+        <f t="shared" ref="F3:F48" si="0">C3-$C$2</f>
         <v>206.65799999999581</v>
       </c>
       <c r="G3" t="s">
@@ -2504,26 +2535,217 @@
       <c r="A56">
         <v>7.1</v>
       </c>
+      <c r="B56" s="1">
+        <v>44686.05</v>
+      </c>
+      <c r="C56" s="1">
+        <v>-381814.02799999999</v>
+      </c>
+      <c r="D56" s="1">
+        <v>17263724</v>
+      </c>
+      <c r="F56">
+        <f t="shared" ref="F56:F65" si="1">C56-$C$2</f>
+        <v>234.43499999999767</v>
+      </c>
+      <c r="J56" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>7.2</v>
       </c>
+      <c r="B57" s="1">
+        <v>41110.71</v>
+      </c>
+      <c r="C57" s="1">
+        <v>-381863.76299999998</v>
+      </c>
+      <c r="D57" s="1">
+        <v>17216428</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="1"/>
+        <v>184.70000000001164</v>
+      </c>
+      <c r="J57" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>7.3</v>
       </c>
+      <c r="B58" s="1">
+        <v>43054.91</v>
+      </c>
+      <c r="C58" s="1">
+        <v>-381819.00799999997</v>
+      </c>
+      <c r="D58" s="1">
+        <v>17215656</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="1"/>
+        <v>229.4550000000163</v>
+      </c>
+      <c r="J58" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>7.4</v>
       </c>
+      <c r="B59" s="1">
+        <v>42813.18</v>
+      </c>
+      <c r="C59" s="1">
+        <v>-381604.049</v>
+      </c>
+      <c r="D59" s="1">
+        <v>17249048</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="1"/>
+        <v>444.41399999998976</v>
+      </c>
+      <c r="G59" t="s">
+        <v>12</v>
+      </c>
+      <c r="J59" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>7.5</v>
       </c>
+      <c r="B60" s="1">
+        <v>45508.95</v>
+      </c>
+      <c r="C60" s="1">
+        <v>-381838.78100000002</v>
+      </c>
+      <c r="D60" s="1">
+        <v>17030732</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="1"/>
+        <v>209.68199999997159</v>
+      </c>
+      <c r="J60" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>8.1</v>
+      </c>
+      <c r="B61" s="1">
+        <v>49349.25</v>
+      </c>
+      <c r="C61" s="1">
+        <v>-381604.049</v>
+      </c>
+      <c r="D61" s="1">
+        <v>17249104</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="1"/>
+        <v>444.41399999998976</v>
+      </c>
+      <c r="J61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="B62" s="1">
+        <v>59482.7</v>
+      </c>
+      <c r="C62" s="1">
+        <v>-381727.15100000001</v>
+      </c>
+      <c r="D62" s="1">
+        <v>17283796</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="1"/>
+        <v>321.31199999997625</v>
+      </c>
+      <c r="J62" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="B63" s="1">
+        <v>44243.49</v>
+      </c>
+      <c r="C63" s="1">
+        <v>-381896.94</v>
+      </c>
+      <c r="D63" s="1">
+        <v>17118112</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="1"/>
+        <v>151.5229999999865</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>8.4</v>
+      </c>
+      <c r="B64" s="1">
+        <v>61263.31</v>
+      </c>
+      <c r="C64" s="1">
+        <v>-381815.42</v>
+      </c>
+      <c r="D64" s="1">
+        <v>17178212</v>
+      </c>
+      <c r="F64">
+        <f t="shared" si="1"/>
+        <v>233.04300000000512</v>
+      </c>
+      <c r="J64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>8.5</v>
+      </c>
+      <c r="B65" s="1">
+        <v>54436.22</v>
+      </c>
+      <c r="C65" s="1">
+        <v>-381714.712</v>
+      </c>
+      <c r="D65" s="1">
+        <v>17648108</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="1"/>
+        <v>333.75099999998929</v>
+      </c>
+      <c r="J65" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D66" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>